<commit_message>
Add bar chart to location report
</commit_message>
<xml_diff>
--- a/database/6973/JobSummary.xlsx
+++ b/database/6973/JobSummary.xlsx
@@ -680,17 +680,17 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -882,9 +882,9 @@
           </dLbls>
           <cat>
             <strRef>
-              <f>'Spool Location'!$A$1:$A$7</f>
+              <f>'Spool Location'!$A$1:$A$9</f>
               <strCache>
-                <ptCount val="7"/>
+                <ptCount val="9"/>
                 <pt idx="0">
                   <v>Not Workable</v>
                 </pt>
@@ -904,17 +904,23 @@
                   <v>Shipped to Coating</v>
                 </pt>
                 <pt idx="6">
+                  <v>Ready To Deliver</v>
+                </pt>
+                <pt idx="7">
                   <v>Delivered</v>
+                </pt>
+                <pt idx="8">
+                  <v>On Hold</v>
                 </pt>
               </strCache>
             </strRef>
           </cat>
           <val>
             <numRef>
-              <f>'Spool Location'!$B$1:$B$7</f>
+              <f>'Spool Location'!$B$1:$B$9</f>
               <numCache>
                 <formatCode>General</formatCode>
-                <ptCount val="7"/>
+                <ptCount val="9"/>
               </numCache>
             </numRef>
           </val>
@@ -3929,10 +3935,10 @@
       <rowOff>0</rowOff>
     </from>
     <to>
-      <col>16</col>
-      <colOff>514350</colOff>
-      <row>35</row>
-      <rowOff>66674</rowOff>
+      <col>19</col>
+      <colOff>447674</colOff>
+      <row>34</row>
+      <rowOff>114300</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -4403,7 +4409,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4418,27 +4424,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="42.75" customFormat="1" customHeight="1" s="47" thickBot="1">
-      <c r="A1" s="55" t="inlineStr">
+      <c r="A1" s="57" t="inlineStr">
         <is>
           <t>MARATHON: 6973</t>
         </is>
       </c>
       <c r="B1" s="61" t="n"/>
-      <c r="C1" s="56" t="inlineStr">
+      <c r="C1" s="58" t="inlineStr">
         <is>
           <t>1773 Spools</t>
         </is>
       </c>
       <c r="D1" s="61" t="n"/>
       <c r="E1" s="49" t="n"/>
-      <c r="F1" s="56" t="inlineStr">
+      <c r="F1" s="58" t="inlineStr">
         <is>
           <t>1773 Workable</t>
         </is>
       </c>
       <c r="G1" s="61" t="n"/>
       <c r="H1" s="49" t="n"/>
-      <c r="I1" s="56" t="inlineStr">
+      <c r="I1" s="58" t="inlineStr">
         <is>
           <t>1773 Issued</t>
         </is>
@@ -4460,13 +4466,13 @@
       <c r="K2" s="47" t="n"/>
     </row>
     <row r="3" ht="24.75" customFormat="1" customHeight="1" s="1">
-      <c r="A3" s="57" t="inlineStr">
+      <c r="A3" s="56" t="inlineStr">
         <is>
           <t>SPOOLS BY SCOPE</t>
         </is>
       </c>
       <c r="F3" s="19" t="n"/>
-      <c r="G3" s="57" t="inlineStr">
+      <c r="G3" s="56" t="inlineStr">
         <is>
           <t>TOTAL PURCHASED (ITEM QUANTITIES)</t>
         </is>
@@ -4860,7 +4866,7 @@
         <v/>
       </c>
       <c r="F14" s="5" t="n"/>
-      <c r="G14" s="57" t="inlineStr">
+      <c r="G14" s="56" t="inlineStr">
         <is>
           <t>TOTAL NO MATERIAL (ITEM QUANTITIES)</t>
         </is>
@@ -4943,7 +4949,7 @@
       </c>
     </row>
     <row r="17" ht="25.15" customFormat="1" customHeight="1" s="1">
-      <c r="A17" s="57" t="inlineStr">
+      <c r="A17" s="56" t="inlineStr">
         <is>
           <t>TOTAL SHORTS (ITEM QUANTITIES)</t>
         </is>
@@ -5239,7 +5245,7 @@
         <v/>
       </c>
       <c r="F25" s="21" t="n"/>
-      <c r="G25" s="57" t="inlineStr">
+      <c r="G25" s="56" t="inlineStr">
         <is>
           <t>SPOOLS MISSING VALVE ONLY</t>
         </is>
@@ -5976,16 +5982,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A3:E3"/>
     <mergeCell ref="A31:N31"/>
     <mergeCell ref="G14:K14"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="G25:K25"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" paperSize="17" scale="88" fitToHeight="0" verticalDpi="0"/>
@@ -8235,7 +8241,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8249,7 +8255,9 @@
           <t>Not Workable</t>
         </is>
       </c>
-      <c r="B1" s="26" t="n"/>
+      <c r="B1" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="inlineStr">
@@ -8257,7 +8265,9 @@
           <t>Workable</t>
         </is>
       </c>
-      <c r="B2" s="26" t="n"/>
+      <c r="B2" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="inlineStr">
@@ -8265,7 +8275,9 @@
           <t>Issued</t>
         </is>
       </c>
-      <c r="B3" s="26" t="n"/>
+      <c r="B3" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="26" t="inlineStr">
@@ -8273,7 +8285,9 @@
           <t>Pulled</t>
         </is>
       </c>
-      <c r="B4" s="26" t="n"/>
+      <c r="B4" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="inlineStr">
@@ -8281,7 +8295,9 @@
           <t>Welded Out</t>
         </is>
       </c>
-      <c r="B5" s="26" t="n"/>
+      <c r="B5" s="26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="inlineStr">
@@ -8289,23 +8305,39 @@
           <t>Shipped to Coating</t>
         </is>
       </c>
-      <c r="B6" s="26" t="n"/>
+      <c r="B6" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="26" t="inlineStr">
         <is>
+          <t>Ready To Deliver</t>
+        </is>
+      </c>
+      <c r="B7" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="inlineStr">
+        <is>
           <t>Delivered</t>
         </is>
       </c>
-      <c r="B7" s="26" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="26" t="n"/>
-      <c r="B8" s="26" t="n"/>
+      <c r="B8" s="26" t="n">
+        <v>1772</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="26" t="n"/>
-      <c r="B9" s="26" t="n"/>
+      <c r="A9" s="26" t="inlineStr">
+        <is>
+          <t>On Hold</t>
+        </is>
+      </c>
+      <c r="B9" s="26" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>